<commit_message>
boxplots, FDR filter for target enriched
</commit_message>
<xml_diff>
--- a/display_items/supplement.xlsx
+++ b/display_items/supplement.xlsx
@@ -6,7 +6,7 @@
     <workbookView xWindow="0" yWindow="0" windowWidth="13125" windowHeight="6105" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="contents" sheetId="24" state="visible" r:id="rId24"/>
+    <sheet name="contents" sheetId="25" state="visible" r:id="rId25"/>
     <sheet name="s01" sheetId="1" state="visible" r:id="rId1"/>
     <sheet name="s02" sheetId="2" state="visible" r:id="rId2"/>
     <sheet name="s03" sheetId="3" state="visible" r:id="rId3"/>
@@ -30,15 +30,16 @@
     <sheet name="s21" sheetId="21" state="visible" r:id="rId21"/>
     <sheet name="s22" sheetId="22" state="visible" r:id="rId22"/>
     <sheet name="s23" sheetId="23" state="visible" r:id="rId23"/>
+    <sheet name="s24" sheetId="24" state="visible" r:id="rId24"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'contents'!$A$1:$B$24</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'contents'!$A$1:$B$25</definedName>
   </definedNames>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="302" uniqueCount="302">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="322" uniqueCount="322">
   <si>
     <t xml:space="preserve">attribute</t>
   </si>
@@ -214,7 +215,7 @@
     <t xml:space="preserve">target_enriched</t>
   </si>
   <si>
-    <t xml:space="preserve">#DEF2D9</t>
+    <t xml:space="preserve">#DEF2D8</t>
   </si>
   <si>
     <t xml:space="preserve">observed</t>
@@ -235,7 +236,7 @@
     <t xml:space="preserve">#B9E3B3</t>
   </si>
   <si>
-    <t xml:space="preserve">#84CB83</t>
+    <t xml:space="preserve">#81CA81</t>
   </si>
   <si>
     <t xml:space="preserve">#4EB163</t>
@@ -244,13 +245,13 @@
     <t xml:space="preserve">#74C476</t>
   </si>
   <si>
-    <t xml:space="preserve">#CDEBC6</t>
+    <t xml:space="preserve">#CCEBC5</t>
   </si>
   <si>
     <t xml:space="preserve">#B5E1AE</t>
   </si>
   <si>
-    <t xml:space="preserve">#B4E1AD</t>
+    <t xml:space="preserve">#B1DFAA</t>
   </si>
   <si>
     <t xml:space="preserve">disp</t>
@@ -607,6 +608,54 @@
     <t xml:space="preserve">max_severity:sim_assocTRUE</t>
   </si>
   <si>
+    <t xml:space="preserve">bin_max</t>
+  </si>
+  <si>
+    <t xml:space="preserve">bin_disp</t>
+  </si>
+  <si>
+    <t xml:space="preserve">n_se</t>
+  </si>
+  <si>
+    <t xml:space="preserve">min_n</t>
+  </si>
+  <si>
+    <t xml:space="preserve">q25_n</t>
+  </si>
+  <si>
+    <t xml:space="preserve">q50_n</t>
+  </si>
+  <si>
+    <t xml:space="preserve">q75_n</t>
+  </si>
+  <si>
+    <t xml:space="preserve">max_n</t>
+  </si>
+  <si>
+    <t xml:space="preserve">iqr</t>
+  </si>
+  <si>
+    <t xml:space="preserve">minwhisk_n</t>
+  </si>
+  <si>
+    <t xml:space="preserve">maxwhisk_n</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.0-0.2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.2-0.4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.4-0.6</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.6-0.8</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.8-1.0</t>
+  </si>
+  <si>
     <t xml:space="preserve">t_value</t>
   </si>
   <si>
@@ -637,6 +686,12 @@
     <t xml:space="preserve">q75_severity</t>
   </si>
   <si>
+    <t xml:space="preserve">minwhisk_severity</t>
+  </si>
+  <si>
+    <t xml:space="preserve">maxwhisk_severity</t>
+  </si>
+  <si>
     <t xml:space="preserve">ALL</t>
   </si>
   <si>
@@ -937,10 +992,16 @@
     <t xml:space="preserve">s22</t>
   </si>
   <si>
+    <t xml:space="preserve">SE drug specificity versus severity bin.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">s23</t>
+  </si>
+  <si>
     <t xml:space="preserve">Linear model coefficients for SE severity vs. drug specificity.</t>
   </si>
   <si>
-    <t xml:space="preserve">s23</t>
+    <t xml:space="preserve">s24</t>
   </si>
   <si>
     <t xml:space="preserve">Breakdown by MeSH area.</t>
@@ -1377,10 +1438,10 @@
         <v>10</v>
       </c>
       <c r="B9" t="n">
-        <v>20193</v>
+        <v>13122</v>
       </c>
       <c r="C9" t="n">
-        <v>0.0170075246484033</v>
+        <v>0.0110519852640196</v>
       </c>
     </row>
   </sheetData>
@@ -3735,57 +3796,216 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="1" t="s">
-        <v>132</v>
+        <v>189</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>133</v>
+        <v>190</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>134</v>
+        <v>191</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>189</v>
+        <v>192</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>190</v>
+        <v>193</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>194</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>195</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>196</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>197</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>198</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>199</v>
       </c>
     </row>
     <row r="2">
-      <c r="A2" t="s">
-        <v>137</v>
-      </c>
-      <c r="B2" t="n">
-        <v>3.13581603674981</v>
+      <c r="A2" t="n">
+        <v>0.2</v>
+      </c>
+      <c r="B2" t="s">
+        <v>200</v>
       </c>
       <c r="C2" t="n">
-        <v>0.175348787142636</v>
+        <v>21</v>
       </c>
       <c r="D2" t="n">
-        <v>17.8833061114874</v>
+        <v>2</v>
       </c>
       <c r="E2" t="n">
-        <v>0.0000000000000000000000000000000000000000000000000000000000000686595929660927</v>
+        <v>11</v>
+      </c>
+      <c r="F2" t="n">
+        <v>32</v>
+      </c>
+      <c r="G2" t="n">
+        <v>53</v>
+      </c>
+      <c r="H2" t="n">
+        <v>311</v>
+      </c>
+      <c r="I2" t="n">
+        <v>42</v>
+      </c>
+      <c r="J2" t="n">
+        <v>2</v>
+      </c>
+      <c r="K2" t="n">
+        <v>111</v>
       </c>
     </row>
     <row r="3">
-      <c r="A3" t="s">
-        <v>186</v>
-      </c>
-      <c r="B3" t="n">
-        <v>-1.13530863443501</v>
+      <c r="A3" t="n">
+        <v>0.4</v>
+      </c>
+      <c r="B3" t="s">
+        <v>201</v>
       </c>
       <c r="C3" t="n">
-        <v>0.305071635802523</v>
+        <v>197</v>
       </c>
       <c r="D3" t="n">
-        <v>-3.72144932926478</v>
+        <v>1</v>
       </c>
       <c r="E3" t="n">
-        <v>0.000209689137289407</v>
+        <v>5</v>
+      </c>
+      <c r="F3" t="n">
+        <v>17</v>
+      </c>
+      <c r="G3" t="n">
+        <v>86</v>
+      </c>
+      <c r="H3" t="n">
+        <v>507</v>
+      </c>
+      <c r="I3" t="n">
+        <v>81</v>
+      </c>
+      <c r="J3" t="n">
+        <v>1</v>
+      </c>
+      <c r="K3" t="n">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="n">
+        <v>0.6</v>
+      </c>
+      <c r="B4" t="s">
+        <v>202</v>
+      </c>
+      <c r="C4" t="n">
+        <v>391</v>
+      </c>
+      <c r="D4" t="n">
+        <v>1</v>
+      </c>
+      <c r="E4" t="n">
+        <v>3</v>
+      </c>
+      <c r="F4" t="n">
+        <v>10</v>
+      </c>
+      <c r="G4" t="n">
+        <v>45</v>
+      </c>
+      <c r="H4" t="n">
+        <v>458</v>
+      </c>
+      <c r="I4" t="n">
+        <v>42</v>
+      </c>
+      <c r="J4" t="n">
+        <v>1</v>
+      </c>
+      <c r="K4" t="n">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="n">
+        <v>0.8</v>
+      </c>
+      <c r="B5" t="s">
+        <v>203</v>
+      </c>
+      <c r="C5" t="n">
+        <v>262</v>
+      </c>
+      <c r="D5" t="n">
+        <v>1</v>
+      </c>
+      <c r="E5" t="n">
+        <v>2</v>
+      </c>
+      <c r="F5" t="n">
+        <v>9.5</v>
+      </c>
+      <c r="G5" t="n">
+        <v>41.25</v>
+      </c>
+      <c r="H5" t="n">
+        <v>445</v>
+      </c>
+      <c r="I5" t="n">
+        <v>39.25</v>
+      </c>
+      <c r="J5" t="n">
+        <v>1</v>
+      </c>
+      <c r="K5" t="n">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="n">
+        <v>1</v>
+      </c>
+      <c r="B6" t="s">
+        <v>204</v>
+      </c>
+      <c r="C6" t="n">
+        <v>83</v>
+      </c>
+      <c r="D6" t="n">
+        <v>1</v>
+      </c>
+      <c r="E6" t="n">
+        <v>2</v>
+      </c>
+      <c r="F6" t="n">
+        <v>9</v>
+      </c>
+      <c r="G6" t="n">
+        <v>43</v>
+      </c>
+      <c r="H6" t="n">
+        <v>260</v>
+      </c>
+      <c r="I6" t="n">
+        <v>41</v>
+      </c>
+      <c r="J6" t="n">
+        <v>1</v>
+      </c>
+      <c r="K6" t="n">
+        <v>93</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:E3"/>
+  <autoFilter ref="A1:K6"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>
 </worksheet>
@@ -3803,22 +4023,90 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="1" t="s">
-        <v>191</v>
+        <v>132</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>192</v>
+        <v>133</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>205</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="s">
+        <v>137</v>
+      </c>
+      <c r="B2" t="n">
+        <v>3.13581603674981</v>
+      </c>
+      <c r="C2" t="n">
+        <v>0.175348787142636</v>
+      </c>
+      <c r="D2" t="n">
+        <v>17.8833061114874</v>
+      </c>
+      <c r="E2" t="n">
+        <v>0.0000000000000000000000000000000000000000000000000000000000000686595929660927</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="s">
+        <v>186</v>
+      </c>
+      <c r="B3" t="n">
+        <v>-1.13530863443501</v>
+      </c>
+      <c r="C3" t="n">
+        <v>0.305071635802523</v>
+      </c>
+      <c r="D3" t="n">
+        <v>-3.72144932926478</v>
+      </c>
+      <c r="E3" t="n">
+        <v>0.000209689137289407</v>
+      </c>
+    </row>
+  </sheetData>
+  <autoFilter ref="A1:E3"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0" zoomScale="100" showGridLines="1" tabSelected="false">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.0" baseColWidth="10"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="s">
+        <v>207</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>208</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>54</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>193</v>
+        <v>209</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>194</v>
+        <v>210</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>195</v>
+        <v>211</v>
       </c>
       <c r="G1" s="1" t="s">
         <v>49</v>
@@ -3857,36 +4145,42 @@
         <v>170</v>
       </c>
       <c r="S1" s="1" t="s">
-        <v>196</v>
+        <v>212</v>
       </c>
       <c r="T1" s="1" t="s">
-        <v>197</v>
+        <v>213</v>
       </c>
       <c r="U1" s="1" t="s">
-        <v>198</v>
+        <v>214</v>
       </c>
       <c r="V1" s="1" t="s">
+        <v>215</v>
+      </c>
+      <c r="W1" s="1" t="s">
+        <v>216</v>
+      </c>
+      <c r="X1" s="1" t="s">
         <v>171</v>
       </c>
-      <c r="W1" s="1" t="s">
+      <c r="Y1" s="1" t="s">
         <v>172</v>
       </c>
-      <c r="X1" s="1" t="s">
+      <c r="Z1" s="1" t="s">
         <v>173</v>
       </c>
-      <c r="Y1" s="1" t="s">
+      <c r="AA1" s="1" t="s">
         <v>174</v>
       </c>
-      <c r="Z1" s="1" t="s">
+      <c r="AB1" s="1" t="s">
         <v>175</v>
       </c>
-      <c r="AA1" s="1" t="s">
+      <c r="AC1" s="1" t="s">
         <v>176</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>199</v>
+        <v>217</v>
       </c>
       <c r="B2" t="s">
         <v>88</v>
@@ -3895,13 +4189,13 @@
         <v>56</v>
       </c>
       <c r="D2" t="s">
-        <v>200</v>
+        <v>218</v>
       </c>
       <c r="E2" t="s">
-        <v>201</v>
+        <v>219</v>
       </c>
       <c r="F2" t="s">
-        <v>202</v>
+        <v>220</v>
       </c>
       <c r="G2" t="n">
         <v>18</v>
@@ -3926,10 +4220,12 @@
       <c r="Y2"/>
       <c r="Z2"/>
       <c r="AA2"/>
+      <c r="AB2"/>
+      <c r="AC2"/>
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>199</v>
+        <v>217</v>
       </c>
       <c r="B3" t="s">
         <v>88</v>
@@ -3938,13 +4234,13 @@
         <v>56</v>
       </c>
       <c r="D3" t="s">
-        <v>200</v>
+        <v>218</v>
       </c>
       <c r="E3" t="s">
-        <v>201</v>
+        <v>219</v>
       </c>
       <c r="F3" t="s">
-        <v>203</v>
+        <v>221</v>
       </c>
       <c r="G3" t="n">
         <v>18</v>
@@ -3992,42 +4288,48 @@
         <v>0.68</v>
       </c>
       <c r="V3" t="n">
+        <v>0.04</v>
+      </c>
+      <c r="W3" t="n">
+        <v>1</v>
+      </c>
+      <c r="X3" t="n">
         <v>0.11178560852828</v>
       </c>
-      <c r="W3" t="n">
+      <c r="Y3" t="n">
         <v>0.104490348322689</v>
       </c>
-      <c r="X3" t="n">
+      <c r="Z3" t="n">
         <v>0.119522225521396</v>
       </c>
-      <c r="Y3" t="n">
+      <c r="AA3" t="n">
         <v>0.940163254851473</v>
       </c>
-      <c r="Z3" t="n">
+      <c r="AB3" t="n">
         <v>0.939621219459967</v>
       </c>
-      <c r="AA3" t="n">
+      <c r="AC3" t="n">
         <v>0.940700731347176</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>204</v>
+        <v>222</v>
       </c>
       <c r="B4" t="s">
-        <v>205</v>
+        <v>223</v>
       </c>
       <c r="C4" t="s">
-        <v>206</v>
+        <v>224</v>
       </c>
       <c r="D4" t="s">
-        <v>207</v>
+        <v>225</v>
       </c>
       <c r="E4" t="s">
-        <v>201</v>
+        <v>219</v>
       </c>
       <c r="F4" t="s">
-        <v>202</v>
+        <v>220</v>
       </c>
       <c r="G4" t="n">
         <v>17</v>
@@ -4075,42 +4377,48 @@
         <v>0.62</v>
       </c>
       <c r="V4" t="n">
+        <v>0.23</v>
+      </c>
+      <c r="W4" t="n">
+        <v>0.86</v>
+      </c>
+      <c r="X4" t="n">
         <v>0.2</v>
       </c>
-      <c r="W4" t="n">
+      <c r="Y4" t="n">
         <v>0.0886058468680258</v>
       </c>
-      <c r="X4" t="n">
+      <c r="Z4" t="n">
         <v>0.391309503695403</v>
       </c>
-      <c r="Y4" t="n">
+      <c r="AA4" t="n">
         <v>0.942965232230606</v>
       </c>
-      <c r="Z4" t="n">
+      <c r="AB4" t="n">
         <v>0.940869012276397</v>
       </c>
-      <c r="AA4" t="n">
+      <c r="AC4" t="n">
         <v>0.944991484945451</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>204</v>
+        <v>222</v>
       </c>
       <c r="B5" t="s">
-        <v>205</v>
+        <v>223</v>
       </c>
       <c r="C5" t="s">
-        <v>206</v>
+        <v>224</v>
       </c>
       <c r="D5" t="s">
-        <v>207</v>
+        <v>225</v>
       </c>
       <c r="E5" t="s">
-        <v>201</v>
+        <v>219</v>
       </c>
       <c r="F5" t="s">
-        <v>203</v>
+        <v>221</v>
       </c>
       <c r="G5" t="n">
         <v>17</v>
@@ -4158,42 +4466,48 @@
         <v>0.62</v>
       </c>
       <c r="V5" t="n">
+        <v>0.23</v>
+      </c>
+      <c r="W5" t="n">
+        <v>0.86</v>
+      </c>
+      <c r="X5" t="n">
         <v>0.2</v>
       </c>
-      <c r="W5" t="n">
+      <c r="Y5" t="n">
         <v>0.0886058468680258</v>
       </c>
-      <c r="X5" t="n">
+      <c r="Z5" t="n">
         <v>0.391309503695403</v>
       </c>
-      <c r="Y5" t="n">
+      <c r="AA5" t="n">
         <v>0.9419536581495</v>
       </c>
-      <c r="Z5" t="n">
+      <c r="AB5" t="n">
         <v>0.939878510107926</v>
       </c>
-      <c r="AA5" t="n">
+      <c r="AC5" t="n">
         <v>0.943961451112216</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>208</v>
+        <v>226</v>
       </c>
       <c r="B6" t="s">
-        <v>209</v>
+        <v>227</v>
       </c>
       <c r="C6" t="s">
         <v>116</v>
       </c>
       <c r="D6" t="s">
-        <v>207</v>
+        <v>225</v>
       </c>
       <c r="E6" t="s">
-        <v>201</v>
+        <v>219</v>
       </c>
       <c r="F6" t="s">
-        <v>202</v>
+        <v>220</v>
       </c>
       <c r="G6" t="n">
         <v>16</v>
@@ -4241,42 +4555,48 @@
         <v>0.86</v>
       </c>
       <c r="V6" t="n">
+        <v>0.27</v>
+      </c>
+      <c r="W6" t="n">
+        <v>0.96</v>
+      </c>
+      <c r="X6" t="n">
         <v>0.107438016528926</v>
       </c>
-      <c r="W6" t="n">
+      <c r="Y6" t="n">
         <v>0.0638696835578645</v>
       </c>
-      <c r="X6" t="n">
+      <c r="Z6" t="n">
         <v>0.175165161938089</v>
       </c>
-      <c r="Y6" t="n">
+      <c r="AA6" t="n">
         <v>0.990057417496744</v>
       </c>
-      <c r="Z6" t="n">
+      <c r="AB6" t="n">
         <v>0.989189328823355</v>
       </c>
-      <c r="AA6" t="n">
+      <c r="AC6" t="n">
         <v>0.990856443644179</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>208</v>
+        <v>226</v>
       </c>
       <c r="B7" t="s">
-        <v>209</v>
+        <v>227</v>
       </c>
       <c r="C7" t="s">
         <v>116</v>
       </c>
       <c r="D7" t="s">
-        <v>207</v>
+        <v>225</v>
       </c>
       <c r="E7" t="s">
-        <v>201</v>
+        <v>219</v>
       </c>
       <c r="F7" t="s">
-        <v>203</v>
+        <v>221</v>
       </c>
       <c r="G7" t="n">
         <v>16</v>
@@ -4324,42 +4644,48 @@
         <v>0.86</v>
       </c>
       <c r="V7" t="n">
+        <v>0.27</v>
+      </c>
+      <c r="W7" t="n">
+        <v>0.96</v>
+      </c>
+      <c r="X7" t="n">
         <v>0.054673721340388</v>
       </c>
-      <c r="W7" t="n">
+      <c r="Y7" t="n">
         <v>0.0387816431675275</v>
       </c>
-      <c r="X7" t="n">
+      <c r="Z7" t="n">
         <v>0.0765594166018811</v>
       </c>
-      <c r="Y7" t="n">
+      <c r="AA7" t="n">
         <v>0.987589672185731</v>
       </c>
-      <c r="Z7" t="n">
+      <c r="AB7" t="n">
         <v>0.986716738193244</v>
       </c>
-      <c r="AA7" t="n">
+      <c r="AC7" t="n">
         <v>0.988405913780108</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>210</v>
+        <v>228</v>
       </c>
       <c r="B8" t="s">
-        <v>211</v>
+        <v>229</v>
       </c>
       <c r="C8" t="s">
-        <v>212</v>
+        <v>230</v>
       </c>
       <c r="D8" t="s">
-        <v>207</v>
+        <v>225</v>
       </c>
       <c r="E8" t="s">
-        <v>201</v>
+        <v>219</v>
       </c>
       <c r="F8" t="s">
-        <v>202</v>
+        <v>220</v>
       </c>
       <c r="G8" t="n">
         <v>15</v>
@@ -4407,42 +4733,48 @@
         <v>0.61</v>
       </c>
       <c r="V8" t="n">
+        <v>0.22</v>
+      </c>
+      <c r="W8" t="n">
+        <v>0.79</v>
+      </c>
+      <c r="X8" t="n">
         <v>0.05</v>
       </c>
-      <c r="W8" t="n">
+      <c r="Y8" t="n">
         <v>0.0300144222382781</v>
       </c>
-      <c r="X8" t="n">
+      <c r="Z8" t="n">
         <v>0.0821660145202883</v>
       </c>
-      <c r="Y8" t="n">
+      <c r="AA8" t="n">
         <v>0.963126843657817</v>
       </c>
-      <c r="Z8" t="n">
+      <c r="AB8" t="n">
         <v>0.961297646160974</v>
       </c>
-      <c r="AA8" t="n">
+      <c r="AC8" t="n">
         <v>0.964872746557466</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>210</v>
+        <v>228</v>
       </c>
       <c r="B9" t="s">
-        <v>211</v>
+        <v>229</v>
       </c>
       <c r="C9" t="s">
-        <v>212</v>
+        <v>230</v>
       </c>
       <c r="D9" t="s">
-        <v>207</v>
+        <v>225</v>
       </c>
       <c r="E9" t="s">
-        <v>201</v>
+        <v>219</v>
       </c>
       <c r="F9" t="s">
-        <v>203</v>
+        <v>221</v>
       </c>
       <c r="G9" t="n">
         <v>15</v>
@@ -4490,42 +4822,48 @@
         <v>0.61</v>
       </c>
       <c r="V9" t="n">
+        <v>0.22</v>
+      </c>
+      <c r="W9" t="n">
+        <v>0.79</v>
+      </c>
+      <c r="X9" t="n">
         <v>0.0564784053156146</v>
       </c>
-      <c r="W9" t="n">
+      <c r="Y9" t="n">
         <v>0.0355579448541335</v>
       </c>
-      <c r="X9" t="n">
+      <c r="Z9" t="n">
         <v>0.0885769381341815</v>
       </c>
-      <c r="Y9" t="n">
+      <c r="AA9" t="n">
         <v>0.961677031953678</v>
       </c>
-      <c r="Z9" t="n">
+      <c r="AB9" t="n">
         <v>0.959896211133048</v>
       </c>
-      <c r="AA9" t="n">
+      <c r="AC9" t="n">
         <v>0.96338179155991</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s">
-        <v>213</v>
+        <v>231</v>
       </c>
       <c r="B10" t="s">
-        <v>214</v>
+        <v>232</v>
       </c>
       <c r="C10" t="s">
-        <v>215</v>
+        <v>233</v>
       </c>
       <c r="D10" t="s">
-        <v>207</v>
+        <v>225</v>
       </c>
       <c r="E10" t="s">
-        <v>201</v>
+        <v>219</v>
       </c>
       <c r="F10" t="s">
-        <v>202</v>
+        <v>220</v>
       </c>
       <c r="G10" t="n">
         <v>14</v>
@@ -4573,42 +4911,48 @@
         <v>0.67</v>
       </c>
       <c r="V10" t="n">
+        <v>0.36</v>
+      </c>
+      <c r="W10" t="n">
+        <v>0.87</v>
+      </c>
+      <c r="X10" t="n">
         <v>0.0618181818181818</v>
       </c>
-      <c r="W10" t="n">
+      <c r="Y10" t="n">
         <v>0.0389509519015554</v>
       </c>
-      <c r="X10" t="n">
+      <c r="Z10" t="n">
         <v>0.0967586336842367</v>
       </c>
-      <c r="Y10" t="n">
+      <c r="AA10" t="n">
         <v>0.94748427672956</v>
       </c>
-      <c r="Z10" t="n">
+      <c r="AB10" t="n">
         <v>0.945571920212677</v>
       </c>
-      <c r="AA10" t="n">
+      <c r="AC10" t="n">
         <v>0.949333042041097</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s">
-        <v>213</v>
+        <v>231</v>
       </c>
       <c r="B11" t="s">
-        <v>214</v>
+        <v>232</v>
       </c>
       <c r="C11" t="s">
-        <v>215</v>
+        <v>233</v>
       </c>
       <c r="D11" t="s">
-        <v>207</v>
+        <v>225</v>
       </c>
       <c r="E11" t="s">
-        <v>201</v>
+        <v>219</v>
       </c>
       <c r="F11" t="s">
-        <v>203</v>
+        <v>221</v>
       </c>
       <c r="G11" t="n">
         <v>14</v>
@@ -4656,42 +5000,48 @@
         <v>0.67</v>
       </c>
       <c r="V11" t="n">
+        <v>0.36</v>
+      </c>
+      <c r="W11" t="n">
+        <v>0.87</v>
+      </c>
+      <c r="X11" t="n">
         <v>0.0602836879432624</v>
       </c>
-      <c r="W11" t="n">
+      <c r="Y11" t="n">
         <v>0.037975337393742</v>
       </c>
-      <c r="X11" t="n">
+      <c r="Z11" t="n">
         <v>0.0944108426125381</v>
       </c>
-      <c r="Y11" t="n">
+      <c r="AA11" t="n">
         <v>0.945589708440976</v>
       </c>
-      <c r="Z11" t="n">
+      <c r="AB11" t="n">
         <v>0.943695731012756</v>
       </c>
-      <c r="AA11" t="n">
+      <c r="AC11" t="n">
         <v>0.947423525275757</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s">
-        <v>216</v>
+        <v>234</v>
       </c>
       <c r="B12" t="s">
-        <v>217</v>
+        <v>235</v>
       </c>
       <c r="C12" t="s">
-        <v>218</v>
+        <v>236</v>
       </c>
       <c r="D12" t="s">
-        <v>207</v>
+        <v>225</v>
       </c>
       <c r="E12" t="s">
-        <v>201</v>
+        <v>219</v>
       </c>
       <c r="F12" t="s">
-        <v>202</v>
+        <v>220</v>
       </c>
       <c r="G12" t="n">
         <v>13</v>
@@ -4739,42 +5089,48 @@
         <v>0.66</v>
       </c>
       <c r="V12" t="n">
+        <v>0.19</v>
+      </c>
+      <c r="W12" t="n">
+        <v>0.93</v>
+      </c>
+      <c r="X12" t="n">
         <v>0.136904761904762</v>
       </c>
-      <c r="W12" t="n">
+      <c r="Y12" t="n">
         <v>0.0929894093373812</v>
       </c>
-      <c r="X12" t="n">
+      <c r="Z12" t="n">
         <v>0.197053861726214</v>
       </c>
-      <c r="Y12" t="n">
+      <c r="AA12" t="n">
         <v>0.91141524623841</v>
       </c>
-      <c r="Z12" t="n">
+      <c r="AB12" t="n">
         <v>0.908436923499763</v>
       </c>
-      <c r="AA12" t="n">
+      <c r="AC12" t="n">
         <v>0.914305830028423</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="s">
-        <v>216</v>
+        <v>234</v>
       </c>
       <c r="B13" t="s">
-        <v>217</v>
+        <v>235</v>
       </c>
       <c r="C13" t="s">
-        <v>218</v>
+        <v>236</v>
       </c>
       <c r="D13" t="s">
-        <v>207</v>
+        <v>225</v>
       </c>
       <c r="E13" t="s">
-        <v>201</v>
+        <v>219</v>
       </c>
       <c r="F13" t="s">
-        <v>203</v>
+        <v>221</v>
       </c>
       <c r="G13" t="n">
         <v>13</v>
@@ -4822,42 +5178,48 @@
         <v>0.66</v>
       </c>
       <c r="V13" t="n">
+        <v>0.19</v>
+      </c>
+      <c r="W13" t="n">
+        <v>0.93</v>
+      </c>
+      <c r="X13" t="n">
         <v>0.138121546961326</v>
       </c>
-      <c r="W13" t="n">
+      <c r="Y13" t="n">
         <v>0.0953373264606933</v>
       </c>
-      <c r="X13" t="n">
+      <c r="Z13" t="n">
         <v>0.195947210916407</v>
       </c>
-      <c r="Y13" t="n">
+      <c r="AA13" t="n">
         <v>0.910919977672908</v>
       </c>
-      <c r="Z13" t="n">
+      <c r="AB13" t="n">
         <v>0.908067538749444</v>
       </c>
-      <c r="AA13" t="n">
+      <c r="AC13" t="n">
         <v>0.913692324327774</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="s">
+        <v>237</v>
+      </c>
+      <c r="B14" t="s">
+        <v>238</v>
+      </c>
+      <c r="C14" t="s">
+        <v>239</v>
+      </c>
+      <c r="D14" t="s">
+        <v>225</v>
+      </c>
+      <c r="E14" t="s">
         <v>219</v>
       </c>
-      <c r="B14" t="s">
+      <c r="F14" t="s">
         <v>220</v>
-      </c>
-      <c r="C14" t="s">
-        <v>221</v>
-      </c>
-      <c r="D14" t="s">
-        <v>207</v>
-      </c>
-      <c r="E14" t="s">
-        <v>201</v>
-      </c>
-      <c r="F14" t="s">
-        <v>202</v>
       </c>
       <c r="G14" t="n">
         <v>12</v>
@@ -4905,42 +5267,48 @@
         <v>0.74</v>
       </c>
       <c r="V14" t="n">
+        <v>0.19</v>
+      </c>
+      <c r="W14" t="n">
+        <v>0.95</v>
+      </c>
+      <c r="X14" t="n">
         <v>0.10126582278481</v>
       </c>
-      <c r="W14" t="n">
+      <c r="Y14" t="n">
         <v>0.0689981335727913</v>
       </c>
-      <c r="X14" t="n">
+      <c r="Z14" t="n">
         <v>0.146253256592927</v>
       </c>
-      <c r="Y14" t="n">
+      <c r="AA14" t="n">
         <v>0.954635901559906</v>
       </c>
-      <c r="Z14" t="n">
+      <c r="AB14" t="n">
         <v>0.953308155366726</v>
       </c>
-      <c r="AA14" t="n">
+      <c r="AC14" t="n">
         <v>0.955927636990922</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="s">
+        <v>237</v>
+      </c>
+      <c r="B15" t="s">
+        <v>238</v>
+      </c>
+      <c r="C15" t="s">
+        <v>239</v>
+      </c>
+      <c r="D15" t="s">
+        <v>225</v>
+      </c>
+      <c r="E15" t="s">
         <v>219</v>
       </c>
-      <c r="B15" t="s">
-        <v>220</v>
-      </c>
-      <c r="C15" t="s">
+      <c r="F15" t="s">
         <v>221</v>
-      </c>
-      <c r="D15" t="s">
-        <v>207</v>
-      </c>
-      <c r="E15" t="s">
-        <v>201</v>
-      </c>
-      <c r="F15" t="s">
-        <v>203</v>
       </c>
       <c r="G15" t="n">
         <v>12</v>
@@ -4988,42 +5356,48 @@
         <v>0.74</v>
       </c>
       <c r="V15" t="n">
+        <v>0.19</v>
+      </c>
+      <c r="W15" t="n">
+        <v>0.95</v>
+      </c>
+      <c r="X15" t="n">
         <v>0.116161616161616</v>
       </c>
-      <c r="W15" t="n">
+      <c r="Y15" t="n">
         <v>0.0882268925398821</v>
       </c>
-      <c r="X15" t="n">
+      <c r="Z15" t="n">
         <v>0.151471759779395</v>
       </c>
-      <c r="Y15" t="n">
+      <c r="AA15" t="n">
         <v>0.946773580924246</v>
       </c>
-      <c r="Z15" t="n">
+      <c r="AB15" t="n">
         <v>0.945480767212496</v>
       </c>
-      <c r="AA15" t="n">
+      <c r="AC15" t="n">
         <v>0.948037423010476</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="s">
-        <v>222</v>
+        <v>240</v>
       </c>
       <c r="B16" t="s">
-        <v>223</v>
+        <v>241</v>
       </c>
       <c r="C16" t="s">
-        <v>224</v>
+        <v>242</v>
       </c>
       <c r="D16" t="s">
-        <v>207</v>
+        <v>225</v>
       </c>
       <c r="E16" t="s">
-        <v>201</v>
+        <v>219</v>
       </c>
       <c r="F16" t="s">
-        <v>202</v>
+        <v>220</v>
       </c>
       <c r="G16" t="n">
         <v>11</v>
@@ -5071,42 +5445,48 @@
         <v>0.59</v>
       </c>
       <c r="V16" t="n">
+        <v>0.19</v>
+      </c>
+      <c r="W16" t="n">
+        <v>0.81</v>
+      </c>
+      <c r="X16" t="n">
         <v>0.062015503875969</v>
       </c>
-      <c r="W16" t="n">
+      <c r="Y16" t="n">
         <v>0.0317561556554095</v>
       </c>
-      <c r="X16" t="n">
+      <c r="Z16" t="n">
         <v>0.117605790508368</v>
       </c>
-      <c r="Y16" t="n">
+      <c r="AA16" t="n">
         <v>0.963441707990124</v>
       </c>
-      <c r="Z16" t="n">
+      <c r="AB16" t="n">
         <v>0.96172893541396</v>
       </c>
-      <c r="AA16" t="n">
+      <c r="AC16" t="n">
         <v>0.9650806108087</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="s">
-        <v>222</v>
+        <v>240</v>
       </c>
       <c r="B17" t="s">
-        <v>223</v>
+        <v>241</v>
       </c>
       <c r="C17" t="s">
-        <v>224</v>
+        <v>242</v>
       </c>
       <c r="D17" t="s">
-        <v>207</v>
+        <v>225</v>
       </c>
       <c r="E17" t="s">
-        <v>201</v>
+        <v>219</v>
       </c>
       <c r="F17" t="s">
-        <v>203</v>
+        <v>221</v>
       </c>
       <c r="G17" t="n">
         <v>11</v>
@@ -5154,42 +5534,48 @@
         <v>0.59</v>
       </c>
       <c r="V17" t="n">
+        <v>0.19</v>
+      </c>
+      <c r="W17" t="n">
+        <v>0.81</v>
+      </c>
+      <c r="X17" t="n">
         <v>0.0671641791044776</v>
       </c>
-      <c r="W17" t="n">
+      <c r="Y17" t="n">
         <v>0.035734606045895</v>
       </c>
-      <c r="X17" t="n">
+      <c r="Z17" t="n">
         <v>0.12271887382554</v>
       </c>
-      <c r="Y17" t="n">
+      <c r="AA17" t="n">
         <v>0.960140096714493</v>
       </c>
-      <c r="Z17" t="n">
+      <c r="AB17" t="n">
         <v>0.958394174499561</v>
       </c>
-      <c r="AA17" t="n">
+      <c r="AC17" t="n">
         <v>0.961815673100767</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="s">
+        <v>243</v>
+      </c>
+      <c r="B18" t="s">
+        <v>244</v>
+      </c>
+      <c r="C18" t="s">
+        <v>245</v>
+      </c>
+      <c r="D18" t="s">
         <v>225</v>
       </c>
-      <c r="B18" t="s">
-        <v>226</v>
-      </c>
-      <c r="C18" t="s">
-        <v>227</v>
-      </c>
-      <c r="D18" t="s">
-        <v>207</v>
-      </c>
       <c r="E18" t="s">
-        <v>201</v>
+        <v>219</v>
       </c>
       <c r="F18" t="s">
-        <v>202</v>
+        <v>220</v>
       </c>
       <c r="G18" t="n">
         <v>10</v>
@@ -5237,42 +5623,48 @@
         <v>0.79</v>
       </c>
       <c r="V18" t="n">
+        <v>0.31</v>
+      </c>
+      <c r="W18" t="n">
+        <v>1</v>
+      </c>
+      <c r="X18" t="n">
         <v>0.278481012658228</v>
       </c>
-      <c r="W18" t="n">
+      <c r="Y18" t="n">
         <v>0.236571288225222</v>
       </c>
-      <c r="X18" t="n">
+      <c r="Z18" t="n">
         <v>0.324657876572628</v>
       </c>
-      <c r="Y18" t="n">
+      <c r="AA18" t="n">
         <v>0.92803743070742</v>
       </c>
-      <c r="Z18" t="n">
+      <c r="AB18" t="n">
         <v>0.925923995104097</v>
       </c>
-      <c r="AA18" t="n">
+      <c r="AC18" t="n">
         <v>0.93009512096527</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="s">
+        <v>243</v>
+      </c>
+      <c r="B19" t="s">
+        <v>244</v>
+      </c>
+      <c r="C19" t="s">
+        <v>245</v>
+      </c>
+      <c r="D19" t="s">
         <v>225</v>
       </c>
-      <c r="B19" t="s">
-        <v>226</v>
-      </c>
-      <c r="C19" t="s">
-        <v>227</v>
-      </c>
-      <c r="D19" t="s">
-        <v>207</v>
-      </c>
       <c r="E19" t="s">
-        <v>201</v>
+        <v>219</v>
       </c>
       <c r="F19" t="s">
-        <v>203</v>
+        <v>221</v>
       </c>
       <c r="G19" t="n">
         <v>10</v>
@@ -5320,42 +5712,48 @@
         <v>0.79</v>
       </c>
       <c r="V19" t="n">
+        <v>0.31</v>
+      </c>
+      <c r="W19" t="n">
+        <v>1</v>
+      </c>
+      <c r="X19" t="n">
         <v>0.277188328912467</v>
       </c>
-      <c r="W19" t="n">
+      <c r="Y19" t="n">
         <v>0.246429437877793</v>
       </c>
-      <c r="X19" t="n">
+      <c r="Z19" t="n">
         <v>0.310206061421938</v>
       </c>
-      <c r="Y19" t="n">
+      <c r="AA19" t="n">
         <v>0.92645823738181</v>
       </c>
-      <c r="Z19" t="n">
+      <c r="AB19" t="n">
         <v>0.924553031124905</v>
       </c>
-      <c r="AA19" t="n">
+      <c r="AC19" t="n">
         <v>0.928319062925262</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="s">
-        <v>228</v>
+        <v>246</v>
       </c>
       <c r="B20" t="s">
-        <v>229</v>
+        <v>247</v>
       </c>
       <c r="C20" t="s">
-        <v>230</v>
+        <v>248</v>
       </c>
       <c r="D20" t="s">
-        <v>207</v>
+        <v>225</v>
       </c>
       <c r="E20" t="s">
-        <v>201</v>
+        <v>219</v>
       </c>
       <c r="F20" t="s">
-        <v>202</v>
+        <v>220</v>
       </c>
       <c r="G20" t="n">
         <v>9</v>
@@ -5403,42 +5801,48 @@
         <v>0.7</v>
       </c>
       <c r="V20" t="n">
+        <v>0.39</v>
+      </c>
+      <c r="W20" t="n">
+        <v>0.83</v>
+      </c>
+      <c r="X20" t="n">
         <v>0.142329020332717</v>
       </c>
-      <c r="W20" t="n">
+      <c r="Y20" t="n">
         <v>0.122774626239996</v>
       </c>
-      <c r="X20" t="n">
+      <c r="Z20" t="n">
         <v>0.164414130725848</v>
       </c>
-      <c r="Y20" t="n">
+      <c r="AA20" t="n">
         <v>0.942947458875522</v>
       </c>
-      <c r="Z20" t="n">
+      <c r="AB20" t="n">
         <v>0.940376437287321</v>
       </c>
-      <c r="AA20" t="n">
+      <c r="AC20" t="n">
         <v>0.945414051060188</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="s">
-        <v>228</v>
+        <v>246</v>
       </c>
       <c r="B21" t="s">
-        <v>229</v>
+        <v>247</v>
       </c>
       <c r="C21" t="s">
-        <v>230</v>
+        <v>248</v>
       </c>
       <c r="D21" t="s">
-        <v>207</v>
+        <v>225</v>
       </c>
       <c r="E21" t="s">
-        <v>201</v>
+        <v>219</v>
       </c>
       <c r="F21" t="s">
-        <v>203</v>
+        <v>221</v>
       </c>
       <c r="G21" t="n">
         <v>9</v>
@@ -5486,42 +5890,48 @@
         <v>0.7</v>
       </c>
       <c r="V21" t="n">
+        <v>0.39</v>
+      </c>
+      <c r="W21" t="n">
+        <v>0.83</v>
+      </c>
+      <c r="X21" t="n">
         <v>0.148614609571788</v>
       </c>
-      <c r="W21" t="n">
+      <c r="Y21" t="n">
         <v>0.12954359923654</v>
       </c>
-      <c r="X21" t="n">
+      <c r="Z21" t="n">
         <v>0.169945053570907</v>
       </c>
-      <c r="Y21" t="n">
+      <c r="AA21" t="n">
         <v>0.942750117980179</v>
       </c>
-      <c r="Z21" t="n">
+      <c r="AB21" t="n">
         <v>0.9402266802334</v>
       </c>
-      <c r="AA21" t="n">
+      <c r="AC21" t="n">
         <v>0.945173236374685</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="s">
-        <v>231</v>
+        <v>249</v>
       </c>
       <c r="B22" t="s">
-        <v>232</v>
+        <v>250</v>
       </c>
       <c r="C22" t="s">
-        <v>233</v>
+        <v>251</v>
       </c>
       <c r="D22" t="s">
-        <v>207</v>
+        <v>225</v>
       </c>
       <c r="E22" t="s">
-        <v>201</v>
+        <v>219</v>
       </c>
       <c r="F22" t="s">
-        <v>202</v>
+        <v>220</v>
       </c>
       <c r="G22" t="n">
         <v>8</v>
@@ -5569,42 +5979,48 @@
         <v>0.7</v>
       </c>
       <c r="V22" t="n">
+        <v>0.13</v>
+      </c>
+      <c r="W22" t="n">
+        <v>0.85</v>
+      </c>
+      <c r="X22" t="n">
         <v>0.049618320610687</v>
       </c>
-      <c r="W22" t="n">
+      <c r="Y22" t="n">
         <v>0.0292233843088209</v>
       </c>
-      <c r="X22" t="n">
+      <c r="Z22" t="n">
         <v>0.0830294559858215</v>
       </c>
-      <c r="Y22" t="n">
+      <c r="AA22" t="n">
         <v>0.989359882958713</v>
       </c>
-      <c r="Z22" t="n">
+      <c r="AB22" t="n">
         <v>0.988446920679762</v>
       </c>
-      <c r="AA22" t="n">
+      <c r="AC22" t="n">
         <v>0.990201415143574</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="s">
-        <v>231</v>
+        <v>249</v>
       </c>
       <c r="B23" t="s">
-        <v>232</v>
+        <v>250</v>
       </c>
       <c r="C23" t="s">
-        <v>233</v>
+        <v>251</v>
       </c>
       <c r="D23" t="s">
-        <v>207</v>
+        <v>225</v>
       </c>
       <c r="E23" t="s">
-        <v>201</v>
+        <v>219</v>
       </c>
       <c r="F23" t="s">
-        <v>203</v>
+        <v>221</v>
       </c>
       <c r="G23" t="n">
         <v>8</v>
@@ -5652,42 +6068,48 @@
         <v>0.7</v>
       </c>
       <c r="V23" t="n">
+        <v>0.13</v>
+      </c>
+      <c r="W23" t="n">
+        <v>0.85</v>
+      </c>
+      <c r="X23" t="n">
         <v>0.0483271375464684</v>
       </c>
-      <c r="W23" t="n">
+      <c r="Y23" t="n">
         <v>0.0284571145425243</v>
       </c>
-      <c r="X23" t="n">
+      <c r="Z23" t="n">
         <v>0.0809157753022896</v>
       </c>
-      <c r="Y23" t="n">
+      <c r="AA23" t="n">
         <v>0.989716129718612</v>
       </c>
-      <c r="Z23" t="n">
+      <c r="AB23" t="n">
         <v>0.988849518507688</v>
       </c>
-      <c r="AA23" t="n">
+      <c r="AC23" t="n">
         <v>0.990516034207055</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="s">
-        <v>234</v>
+        <v>252</v>
       </c>
       <c r="B24" t="s">
-        <v>235</v>
+        <v>253</v>
       </c>
       <c r="C24" t="s">
-        <v>236</v>
+        <v>254</v>
       </c>
       <c r="D24" t="s">
-        <v>207</v>
+        <v>225</v>
       </c>
       <c r="E24" t="s">
-        <v>201</v>
+        <v>219</v>
       </c>
       <c r="F24" t="s">
-        <v>202</v>
+        <v>220</v>
       </c>
       <c r="G24" t="n">
         <v>7</v>
@@ -5735,42 +6157,48 @@
         <v>0.51</v>
       </c>
       <c r="V24" t="n">
+        <v>0.08</v>
+      </c>
+      <c r="W24" t="n">
+        <v>0.77</v>
+      </c>
+      <c r="X24" t="n">
         <v>0.0654205607476635</v>
       </c>
-      <c r="W24" t="n">
+      <c r="Y24" t="n">
         <v>0.0320483042881308</v>
       </c>
-      <c r="X24" t="n">
+      <c r="Z24" t="n">
         <v>0.128915463335641</v>
       </c>
-      <c r="Y24" t="n">
+      <c r="AA24" t="n">
         <v>0.922546788062721</v>
       </c>
-      <c r="Z24" t="n">
+      <c r="AB24" t="n">
         <v>0.920438064148845</v>
       </c>
-      <c r="AA24" t="n">
+      <c r="AC24" t="n">
         <v>0.924604200092116</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="s">
-        <v>234</v>
+        <v>252</v>
       </c>
       <c r="B25" t="s">
-        <v>235</v>
+        <v>253</v>
       </c>
       <c r="C25" t="s">
-        <v>236</v>
+        <v>254</v>
       </c>
       <c r="D25" t="s">
-        <v>207</v>
+        <v>225</v>
       </c>
       <c r="E25" t="s">
-        <v>201</v>
+        <v>219</v>
       </c>
       <c r="F25" t="s">
-        <v>203</v>
+        <v>221</v>
       </c>
       <c r="G25" t="n">
         <v>7</v>
@@ -5818,42 +6246,48 @@
         <v>0.51</v>
       </c>
       <c r="V25" t="n">
+        <v>0.08</v>
+      </c>
+      <c r="W25" t="n">
+        <v>0.77</v>
+      </c>
+      <c r="X25" t="n">
         <v>0.0636363636363636</v>
       </c>
-      <c r="W25" t="n">
+      <c r="Y25" t="n">
         <v>0.0311645180144776</v>
       </c>
-      <c r="X25" t="n">
+      <c r="Z25" t="n">
         <v>0.125557461882102</v>
       </c>
-      <c r="Y25" t="n">
+      <c r="AA25" t="n">
         <v>0.920973247036497</v>
       </c>
-      <c r="Z25" t="n">
+      <c r="AB25" t="n">
         <v>0.918960379696981</v>
       </c>
-      <c r="AA25" t="n">
+      <c r="AC25" t="n">
         <v>0.922940311052999</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="s">
-        <v>237</v>
+        <v>255</v>
       </c>
       <c r="B26" t="s">
-        <v>238</v>
+        <v>256</v>
       </c>
       <c r="C26" t="s">
-        <v>239</v>
+        <v>257</v>
       </c>
       <c r="D26" t="s">
-        <v>207</v>
+        <v>225</v>
       </c>
       <c r="E26" t="s">
-        <v>201</v>
+        <v>219</v>
       </c>
       <c r="F26" t="s">
-        <v>202</v>
+        <v>220</v>
       </c>
       <c r="G26" t="n">
         <v>6</v>
@@ -5901,42 +6335,48 @@
         <v>0.57</v>
       </c>
       <c r="V26" t="n">
+        <v>0.26</v>
+      </c>
+      <c r="W26" t="n">
+        <v>0.77</v>
+      </c>
+      <c r="X26" t="n">
         <v>0.0577507598784195</v>
       </c>
-      <c r="W26" t="n">
+      <c r="Y26" t="n">
         <v>0.0423613830198749</v>
       </c>
-      <c r="X26" t="n">
+      <c r="Z26" t="n">
         <v>0.0782739409789572</v>
       </c>
-      <c r="Y26" t="n">
+      <c r="AA26" t="n">
         <v>0.956237034815426</v>
       </c>
-      <c r="Z26" t="n">
+      <c r="AB26" t="n">
         <v>0.954188406577272</v>
       </c>
-      <c r="AA26" t="n">
+      <c r="AC26" t="n">
         <v>0.958198064766653</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="s">
-        <v>237</v>
+        <v>255</v>
       </c>
       <c r="B27" t="s">
-        <v>238</v>
+        <v>256</v>
       </c>
       <c r="C27" t="s">
-        <v>239</v>
+        <v>257</v>
       </c>
       <c r="D27" t="s">
-        <v>207</v>
+        <v>225</v>
       </c>
       <c r="E27" t="s">
-        <v>201</v>
+        <v>219</v>
       </c>
       <c r="F27" t="s">
-        <v>203</v>
+        <v>221</v>
       </c>
       <c r="G27" t="n">
         <v>6</v>
@@ -5984,42 +6424,48 @@
         <v>0.57</v>
       </c>
       <c r="V27" t="n">
+        <v>0.26</v>
+      </c>
+      <c r="W27" t="n">
+        <v>0.77</v>
+      </c>
+      <c r="X27" t="n">
         <v>0.068287037037037</v>
       </c>
-      <c r="W27" t="n">
+      <c r="Y27" t="n">
         <v>0.0533077602343556</v>
       </c>
-      <c r="X27" t="n">
+      <c r="Z27" t="n">
         <v>0.0870882275146785</v>
       </c>
-      <c r="Y27" t="n">
+      <c r="AA27" t="n">
         <v>0.956990647310288</v>
       </c>
-      <c r="Z27" t="n">
+      <c r="AB27" t="n">
         <v>0.955099934289955</v>
       </c>
-      <c r="AA27" t="n">
+      <c r="AC27" t="n">
         <v>0.958805177598304</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="s">
-        <v>240</v>
+        <v>258</v>
       </c>
       <c r="B28" t="s">
-        <v>241</v>
+        <v>259</v>
       </c>
       <c r="C28" t="s">
-        <v>242</v>
+        <v>260</v>
       </c>
       <c r="D28" t="s">
-        <v>207</v>
+        <v>225</v>
       </c>
       <c r="E28" t="s">
-        <v>201</v>
+        <v>219</v>
       </c>
       <c r="F28" t="s">
-        <v>202</v>
+        <v>220</v>
       </c>
       <c r="G28" t="n">
         <v>5</v>
@@ -6067,42 +6513,48 @@
         <v>0.59</v>
       </c>
       <c r="V28" t="n">
+        <v>0.4</v>
+      </c>
+      <c r="W28" t="n">
+        <v>0.72</v>
+      </c>
+      <c r="X28" t="n">
         <v>0.0824742268041237</v>
       </c>
-      <c r="W28" t="n">
+      <c r="Y28" t="n">
         <v>0.0560469314787348</v>
       </c>
-      <c r="X28" t="n">
+      <c r="Z28" t="n">
         <v>0.119781322214112</v>
       </c>
-      <c r="Y28" t="n">
+      <c r="AA28" t="n">
         <v>0.983215511182769</v>
       </c>
-      <c r="Z28" t="n">
+      <c r="AB28" t="n">
         <v>0.981518204203939</v>
       </c>
-      <c r="AA28" t="n">
+      <c r="AC28" t="n">
         <v>0.984759363472046</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="s">
-        <v>240</v>
+        <v>258</v>
       </c>
       <c r="B29" t="s">
-        <v>241</v>
+        <v>259</v>
       </c>
       <c r="C29" t="s">
-        <v>242</v>
+        <v>260</v>
       </c>
       <c r="D29" t="s">
-        <v>207</v>
+        <v>225</v>
       </c>
       <c r="E29" t="s">
-        <v>201</v>
+        <v>219</v>
       </c>
       <c r="F29" t="s">
-        <v>203</v>
+        <v>221</v>
       </c>
       <c r="G29" t="n">
         <v>5</v>
@@ -6150,42 +6602,48 @@
         <v>0.59</v>
       </c>
       <c r="V29" t="n">
+        <v>0.4</v>
+      </c>
+      <c r="W29" t="n">
+        <v>0.72</v>
+      </c>
+      <c r="X29" t="n">
         <v>0.104712041884817</v>
       </c>
-      <c r="W29" t="n">
+      <c r="Y29" t="n">
         <v>0.0778442584094672</v>
       </c>
-      <c r="X29" t="n">
+      <c r="Z29" t="n">
         <v>0.139450842736354</v>
       </c>
-      <c r="Y29" t="n">
+      <c r="AA29" t="n">
         <v>0.982434503120679</v>
       </c>
-      <c r="Z29" t="n">
+      <c r="AB29" t="n">
         <v>0.980789816686414</v>
       </c>
-      <c r="AA29" t="n">
+      <c r="AC29" t="n">
         <v>0.983940684771357</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="s">
-        <v>243</v>
+        <v>261</v>
       </c>
       <c r="B30" t="s">
-        <v>244</v>
+        <v>262</v>
       </c>
       <c r="C30" t="s">
-        <v>245</v>
+        <v>263</v>
       </c>
       <c r="D30" t="s">
-        <v>207</v>
+        <v>225</v>
       </c>
       <c r="E30" t="s">
-        <v>201</v>
+        <v>219</v>
       </c>
       <c r="F30" t="s">
-        <v>202</v>
+        <v>220</v>
       </c>
       <c r="G30" t="n">
         <v>4</v>
@@ -6233,42 +6691,48 @@
         <v>0.71</v>
       </c>
       <c r="V30" t="n">
+        <v>0.22</v>
+      </c>
+      <c r="W30" t="n">
+        <v>0.87</v>
+      </c>
+      <c r="X30" t="n">
         <v>0.0964912280701754</v>
       </c>
-      <c r="W30" t="n">
+      <c r="Y30" t="n">
         <v>0.0645866008224103</v>
       </c>
-      <c r="X30" t="n">
+      <c r="Z30" t="n">
         <v>0.141767599431715</v>
       </c>
-      <c r="Y30" t="n">
+      <c r="AA30" t="n">
         <v>0.932852126414358</v>
       </c>
-      <c r="Z30" t="n">
+      <c r="AB30" t="n">
         <v>0.929722749327472</v>
       </c>
-      <c r="AA30" t="n">
+      <c r="AC30" t="n">
         <v>0.93585177002983</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="s">
-        <v>243</v>
+        <v>261</v>
       </c>
       <c r="B31" t="s">
-        <v>244</v>
+        <v>262</v>
       </c>
       <c r="C31" t="s">
-        <v>245</v>
+        <v>263</v>
       </c>
       <c r="D31" t="s">
-        <v>207</v>
+        <v>225</v>
       </c>
       <c r="E31" t="s">
-        <v>201</v>
+        <v>219</v>
       </c>
       <c r="F31" t="s">
-        <v>203</v>
+        <v>221</v>
       </c>
       <c r="G31" t="n">
         <v>4</v>
@@ -6316,42 +6780,48 @@
         <v>0.71</v>
       </c>
       <c r="V31" t="n">
+        <v>0.22</v>
+      </c>
+      <c r="W31" t="n">
+        <v>0.87</v>
+      </c>
+      <c r="X31" t="n">
         <v>0.0984251968503937</v>
       </c>
-      <c r="W31" t="n">
+      <c r="Y31" t="n">
         <v>0.0675589766508955</v>
       </c>
-      <c r="X31" t="n">
+      <c r="Z31" t="n">
         <v>0.141257165900237</v>
       </c>
-      <c r="Y31" t="n">
+      <c r="AA31" t="n">
         <v>0.93120442884148</v>
       </c>
-      <c r="Z31" t="n">
+      <c r="AB31" t="n">
         <v>0.928265932349998</v>
       </c>
-      <c r="AA31" t="n">
+      <c r="AC31" t="n">
         <v>0.93403110793587</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="s">
-        <v>246</v>
+        <v>264</v>
       </c>
       <c r="B32" t="s">
-        <v>247</v>
+        <v>265</v>
       </c>
       <c r="C32" t="s">
-        <v>248</v>
+        <v>266</v>
       </c>
       <c r="D32" t="s">
-        <v>207</v>
+        <v>225</v>
       </c>
       <c r="E32" t="s">
-        <v>201</v>
+        <v>219</v>
       </c>
       <c r="F32" t="s">
-        <v>202</v>
+        <v>220</v>
       </c>
       <c r="G32" t="n">
         <v>3</v>
@@ -6399,42 +6869,48 @@
         <v>0.66</v>
       </c>
       <c r="V32" t="n">
+        <v>0.11</v>
+      </c>
+      <c r="W32" t="n">
+        <v>0.95</v>
+      </c>
+      <c r="X32" t="n">
         <v>0.147798742138365</v>
       </c>
-      <c r="W32" t="n">
+      <c r="Y32" t="n">
         <v>0.122333005716924</v>
       </c>
-      <c r="X32" t="n">
+      <c r="Z32" t="n">
         <v>0.177493546901722</v>
       </c>
-      <c r="Y32" t="n">
+      <c r="AA32" t="n">
         <v>0.889436592964061</v>
       </c>
-      <c r="Z32" t="n">
+      <c r="AB32" t="n">
         <v>0.887528183400301</v>
       </c>
-      <c r="AA32" t="n">
+      <c r="AC32" t="n">
         <v>0.891316586183032</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="s">
-        <v>246</v>
+        <v>264</v>
       </c>
       <c r="B33" t="s">
-        <v>247</v>
+        <v>265</v>
       </c>
       <c r="C33" t="s">
-        <v>248</v>
+        <v>266</v>
       </c>
       <c r="D33" t="s">
-        <v>207</v>
+        <v>225</v>
       </c>
       <c r="E33" t="s">
-        <v>201</v>
+        <v>219</v>
       </c>
       <c r="F33" t="s">
-        <v>203</v>
+        <v>221</v>
       </c>
       <c r="G33" t="n">
         <v>3</v>
@@ -6482,42 +6958,48 @@
         <v>0.66</v>
       </c>
       <c r="V33" t="n">
+        <v>0.11</v>
+      </c>
+      <c r="W33" t="n">
+        <v>0.95</v>
+      </c>
+      <c r="X33" t="n">
         <v>0.179287305122494</v>
       </c>
-      <c r="W33" t="n">
+      <c r="Y33" t="n">
         <v>0.155580828842152</v>
       </c>
-      <c r="X33" t="n">
+      <c r="Z33" t="n">
         <v>0.205725979171294</v>
       </c>
-      <c r="Y33" t="n">
+      <c r="AA33" t="n">
         <v>0.888953707834323</v>
       </c>
-      <c r="Z33" t="n">
+      <c r="AB33" t="n">
         <v>0.887330189211333</v>
       </c>
-      <c r="AA33" t="n">
+      <c r="AC33" t="n">
         <v>0.890556717754658</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="s">
-        <v>249</v>
+        <v>267</v>
       </c>
       <c r="B34" t="s">
-        <v>250</v>
+        <v>268</v>
       </c>
       <c r="C34" t="s">
         <v>115</v>
       </c>
       <c r="D34" t="s">
-        <v>207</v>
+        <v>225</v>
       </c>
       <c r="E34" t="s">
-        <v>201</v>
+        <v>219</v>
       </c>
       <c r="F34" t="s">
-        <v>202</v>
+        <v>220</v>
       </c>
       <c r="G34" t="n">
         <v>2</v>
@@ -6565,42 +7047,48 @@
         <v>0.54</v>
       </c>
       <c r="V34" t="n">
+        <v>0.14</v>
+      </c>
+      <c r="W34" t="n">
+        <v>0.82</v>
+      </c>
+      <c r="X34" t="n">
         <v>0.108753315649867</v>
       </c>
-      <c r="W34" t="n">
+      <c r="Y34" t="n">
         <v>0.081183949012351</v>
       </c>
-      <c r="X34" t="n">
+      <c r="Z34" t="n">
         <v>0.144215510086742</v>
       </c>
-      <c r="Y34" t="n">
+      <c r="AA34" t="n">
         <v>0.948251387275778</v>
       </c>
-      <c r="Z34" t="n">
+      <c r="AB34" t="n">
         <v>0.946000885558262</v>
       </c>
-      <c r="AA34" t="n">
+      <c r="AC34" t="n">
         <v>0.950413012052424</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="s">
-        <v>249</v>
+        <v>267</v>
       </c>
       <c r="B35" t="s">
-        <v>250</v>
+        <v>268</v>
       </c>
       <c r="C35" t="s">
         <v>115</v>
       </c>
       <c r="D35" t="s">
-        <v>207</v>
+        <v>225</v>
       </c>
       <c r="E35" t="s">
-        <v>201</v>
+        <v>219</v>
       </c>
       <c r="F35" t="s">
-        <v>203</v>
+        <v>221</v>
       </c>
       <c r="G35" t="n">
         <v>2</v>
@@ -6648,42 +7136,48 @@
         <v>0.54</v>
       </c>
       <c r="V35" t="n">
+        <v>0.14</v>
+      </c>
+      <c r="W35" t="n">
+        <v>0.82</v>
+      </c>
+      <c r="X35" t="n">
         <v>0.14576802507837</v>
       </c>
-      <c r="W35" t="n">
+      <c r="Y35" t="n">
         <v>0.120506513915397</v>
       </c>
-      <c r="X35" t="n">
+      <c r="Z35" t="n">
         <v>0.175269734582955</v>
       </c>
-      <c r="Y35" t="n">
+      <c r="AA35" t="n">
         <v>0.934878978632858</v>
       </c>
-      <c r="Z35" t="n">
+      <c r="AB35" t="n">
         <v>0.932564969194835</v>
       </c>
-      <c r="AA35" t="n">
+      <c r="AC35" t="n">
         <v>0.937118937735844</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="s">
-        <v>251</v>
+        <v>269</v>
       </c>
       <c r="B36" t="s">
-        <v>252</v>
+        <v>270</v>
       </c>
       <c r="C36" t="s">
-        <v>253</v>
+        <v>271</v>
       </c>
       <c r="D36" t="s">
-        <v>207</v>
+        <v>225</v>
       </c>
       <c r="E36" t="s">
-        <v>201</v>
+        <v>219</v>
       </c>
       <c r="F36" t="s">
-        <v>202</v>
+        <v>220</v>
       </c>
       <c r="G36" t="n">
         <v>1</v>
@@ -6731,42 +7225,48 @@
         <v>0.55</v>
       </c>
       <c r="V36" t="n">
+        <v>0.13</v>
+      </c>
+      <c r="W36" t="n">
+        <v>0.8</v>
+      </c>
+      <c r="X36" t="n">
         <v>0.0497237569060773</v>
       </c>
-      <c r="W36" t="n">
+      <c r="Y36" t="n">
         <v>0.038308202193261</v>
       </c>
-      <c r="X36" t="n">
+      <c r="Z36" t="n">
         <v>0.0643135671618126</v>
       </c>
-      <c r="Y36" t="n">
+      <c r="AA36" t="n">
         <v>0.95675597355041</v>
       </c>
-      <c r="Z36" t="n">
+      <c r="AB36" t="n">
         <v>0.955285812036035</v>
       </c>
-      <c r="AA36" t="n">
+      <c r="AC36" t="n">
         <v>0.958179913602559</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="s">
-        <v>251</v>
+        <v>269</v>
       </c>
       <c r="B37" t="s">
-        <v>252</v>
+        <v>270</v>
       </c>
       <c r="C37" t="s">
-        <v>253</v>
+        <v>271</v>
       </c>
       <c r="D37" t="s">
-        <v>207</v>
+        <v>225</v>
       </c>
       <c r="E37" t="s">
-        <v>201</v>
+        <v>219</v>
       </c>
       <c r="F37" t="s">
-        <v>203</v>
+        <v>221</v>
       </c>
       <c r="G37" t="n">
         <v>1</v>
@@ -6814,32 +7314,38 @@
         <v>0.55</v>
       </c>
       <c r="V37" t="n">
+        <v>0.13</v>
+      </c>
+      <c r="W37" t="n">
+        <v>0.8</v>
+      </c>
+      <c r="X37" t="n">
         <v>0.0459183673469388</v>
       </c>
-      <c r="W37" t="n">
+      <c r="Y37" t="n">
         <v>0.0353624137875863</v>
       </c>
-      <c r="X37" t="n">
+      <c r="Z37" t="n">
         <v>0.0594312196998187</v>
       </c>
-      <c r="Y37" t="n">
+      <c r="AA37" t="n">
         <v>0.957291999952599</v>
       </c>
-      <c r="Z37" t="n">
+      <c r="AB37" t="n">
         <v>0.955906827737659</v>
       </c>
-      <c r="AA37" t="n">
+      <c r="AC37" t="n">
         <v>0.958635540436975</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:AA37"/>
+  <autoFilter ref="A1:AC37"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3">
   <dimension ref="A1"/>
   <sheetViews>
@@ -6851,198 +7357,206 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="1" t="s">
-        <v>254</v>
+        <v>272</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>255</v>
+        <v>273</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>256</v>
+        <v>274</v>
       </c>
       <c r="B2" t="s">
-        <v>257</v>
+        <v>275</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>258</v>
+        <v>276</v>
       </c>
       <c r="B3" t="s">
-        <v>259</v>
+        <v>277</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>260</v>
+        <v>278</v>
       </c>
       <c r="B4" t="s">
-        <v>261</v>
+        <v>279</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>262</v>
+        <v>280</v>
       </c>
       <c r="B5" t="s">
-        <v>263</v>
+        <v>281</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>264</v>
+        <v>282</v>
       </c>
       <c r="B6" t="s">
-        <v>265</v>
+        <v>283</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>266</v>
+        <v>284</v>
       </c>
       <c r="B7" t="s">
-        <v>267</v>
+        <v>285</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>268</v>
+        <v>286</v>
       </c>
       <c r="B8" t="s">
-        <v>269</v>
+        <v>287</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>270</v>
+        <v>288</v>
       </c>
       <c r="B9" t="s">
-        <v>271</v>
+        <v>289</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s">
-        <v>272</v>
+        <v>290</v>
       </c>
       <c r="B10" t="s">
-        <v>273</v>
+        <v>291</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s">
-        <v>274</v>
+        <v>292</v>
       </c>
       <c r="B11" t="s">
-        <v>275</v>
+        <v>293</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s">
-        <v>276</v>
+        <v>294</v>
       </c>
       <c r="B12" t="s">
-        <v>277</v>
+        <v>295</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="s">
-        <v>278</v>
+        <v>296</v>
       </c>
       <c r="B13" t="s">
-        <v>279</v>
+        <v>297</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="s">
-        <v>280</v>
+        <v>298</v>
       </c>
       <c r="B14" t="s">
-        <v>281</v>
+        <v>299</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="s">
-        <v>282</v>
+        <v>300</v>
       </c>
       <c r="B15" t="s">
-        <v>283</v>
+        <v>301</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="s">
-        <v>284</v>
+        <v>302</v>
       </c>
       <c r="B16" t="s">
-        <v>285</v>
+        <v>303</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="s">
-        <v>286</v>
+        <v>304</v>
       </c>
       <c r="B17" t="s">
-        <v>287</v>
+        <v>305</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="s">
-        <v>288</v>
+        <v>306</v>
       </c>
       <c r="B18" t="s">
-        <v>289</v>
+        <v>307</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="s">
-        <v>290</v>
+        <v>308</v>
       </c>
       <c r="B19" t="s">
-        <v>291</v>
+        <v>309</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="s">
-        <v>292</v>
+        <v>310</v>
       </c>
       <c r="B20" t="s">
-        <v>293</v>
+        <v>311</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="s">
-        <v>294</v>
+        <v>312</v>
       </c>
       <c r="B21" t="s">
-        <v>295</v>
+        <v>313</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="s">
-        <v>296</v>
+        <v>314</v>
       </c>
       <c r="B22" t="s">
-        <v>297</v>
+        <v>315</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="s">
-        <v>298</v>
+        <v>316</v>
       </c>
       <c r="B23" t="s">
-        <v>299</v>
+        <v>317</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="s">
-        <v>300</v>
+        <v>318</v>
       </c>
       <c r="B24" t="s">
-        <v>301</v>
+        <v>319</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="s">
+        <v>320</v>
+      </c>
+      <c r="B25" t="s">
+        <v>321</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:B24"/>
+  <autoFilter ref="A1:B25"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>
 </worksheet>
@@ -7413,13 +7927,13 @@
         <v>1</v>
       </c>
       <c r="E3" t="n">
-        <v>1.27671471603705</v>
+        <v>1.29739939755774</v>
       </c>
       <c r="F3" t="n">
-        <v>0.000000000000000000000000000000000000000000000000000000000051880705149337</v>
+        <v>0.0000000000000000000000000000000000000000000406697147221778</v>
       </c>
       <c r="G3" t="n">
-        <v>13847</v>
+        <v>9047</v>
       </c>
       <c r="H3" t="n">
         <v>1</v>
@@ -7558,13 +8072,13 @@
         <v>1</v>
       </c>
       <c r="E8" t="n">
-        <v>20.9940711994291</v>
+        <v>22.162880395508</v>
       </c>
       <c r="F8" t="n">
         <v>0</v>
       </c>
       <c r="G8" t="n">
-        <v>10215</v>
+        <v>6993</v>
       </c>
       <c r="H8" t="n">
         <v>3</v>
@@ -7674,13 +8188,13 @@
         <v>1</v>
       </c>
       <c r="E12" t="n">
-        <v>2.47037836125434</v>
+        <v>2.56963102463367</v>
       </c>
       <c r="F12" t="n">
-        <v>0.00000000000000000000000000000000000000169613425400531</v>
+        <v>0.0000000000000000000000000000148255471982314</v>
       </c>
       <c r="G12" t="n">
-        <v>288</v>
+        <v>196</v>
       </c>
       <c r="H12" t="n">
         <v>1</v>
@@ -7761,13 +8275,13 @@
         <v>1</v>
       </c>
       <c r="E15" t="n">
-        <v>5.56908851521439</v>
+        <v>6.13161703308729</v>
       </c>
       <c r="F15" t="n">
-        <v>0.00000000000000000000000000000000000000000000000000000000000316917482330576</v>
+        <v>0.00000000000000000000000000000000000000000000000105651996394744</v>
       </c>
       <c r="G15" t="n">
-        <v>155</v>
+        <v>113</v>
       </c>
       <c r="H15" t="n">
         <v>2</v>
@@ -7796,7 +8310,7 @@
         <v>0</v>
       </c>
       <c r="G16" t="n">
-        <v>20193</v>
+        <v>13122</v>
       </c>
       <c r="H16" t="e">
         <v>#NUM!</v>

</xml_diff>